<commit_message>
all word count done in excel
</commit_message>
<xml_diff>
--- a/TP2/expermiments.xlsx
+++ b/TP2/expermiments.xlsx
@@ -8,32 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beding/Polytechnique/LOG8415E/Laboratoires/LOG8415/TP2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8E20D3-FA2A-B74C-8760-16846816C3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0BE738-6080-C547-AC21-DC662068006A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20440" xr2:uid="{96923936-A141-844A-8B93-6ABFCA660DBE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20400" xr2:uid="{96923936-A141-844A-8B93-6ABFCA660DBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$A$18:$A$26</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$B$17</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$B$18:$B$26</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$C$17</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$C$18:$C$26</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$D$17</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$D$18:$D$26</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Feuil1!$E$17</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Feuil1!$E$18:$E$26</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Feuil1!$B$17</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Feuil1!$B$18:$B$26</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">Feuil1!$C$17</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">Feuil1!$C$18:$C$26</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">Feuil1!$D$17</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">Feuil1!$D$18:$D$26</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">Feuil1!$E$17</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">Feuil1!$E$18:$E$26</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">Feuil1!$A$18:$A$26</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Feuil1!$B$51</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Feuil1!$B$52:$B$60</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Feuil1!$C$51</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Feuil1!$C$52:$C$60</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Feuil1!$D$51</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Feuil1!$D$52:$D$60</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Feuil1!$E$51</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Feuil1!$E$52:$E$60</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Feuil1!$A$52:$A$60</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Feuil1!$A$52:$A$60</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Feuil1!$B$51</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Feuil1!$B$52:$B$60</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Feuil1!$C$51</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Feuil1!$C$52:$C$60</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Feuil1!$D$51</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Feuil1!$D$52:$D$60</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Feuil1!$E$51</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">Feuil1!$E$52:$E$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>dataset/buchanj-midwinter-00-t.txt</t>
   </si>
@@ -95,13 +95,25 @@
   <si>
     <t>Average</t>
   </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>Hadoop</t>
+  </si>
+  <si>
+    <t>Spark on Azure</t>
+  </si>
+  <si>
+    <t>Hadoop on Azure</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -149,7 +161,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -194,7 +206,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$1</c:f>
+              <c:f>Feuil1!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -215,7 +227,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
+              <c:f>Feuil1!$A$3:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -250,7 +262,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$2:$E$10</c:f>
+              <c:f>Feuil1!$E$3:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -295,7 +307,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$D$1</c:f>
+              <c:f>Feuil1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +328,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
+              <c:f>Feuil1!$A$3:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -351,7 +363,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$D$2:$D$10</c:f>
+              <c:f>Feuil1!$D$3:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -396,7 +408,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$1</c:f>
+              <c:f>Feuil1!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -417,7 +429,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
+              <c:f>Feuil1!$A$3:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -452,7 +464,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$2:$C$10</c:f>
+              <c:f>Feuil1!$C$3:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -497,7 +509,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$B$1</c:f>
+              <c:f>Feuil1!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -518,7 +530,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
+              <c:f>Feuil1!$A$3:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -553,7 +565,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$B$10</c:f>
+              <c:f>Feuil1!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -814,7 +826,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$E$17</c:f>
+              <c:f>Feuil1!$E$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -835,7 +847,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$18:$A$26</c:f>
+              <c:f>Feuil1!$A$19:$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -870,7 +882,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$E$18:$E$26</c:f>
+              <c:f>Feuil1!$E$19:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -915,7 +927,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$D$17</c:f>
+              <c:f>Feuil1!$D$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -936,7 +948,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$18:$A$26</c:f>
+              <c:f>Feuil1!$A$19:$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -971,7 +983,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$D$18:$D$26</c:f>
+              <c:f>Feuil1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1016,7 +1028,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$17</c:f>
+              <c:f>Feuil1!$C$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1037,7 +1049,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$18:$A$26</c:f>
+              <c:f>Feuil1!$A$19:$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1072,7 +1084,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$18:$C$26</c:f>
+              <c:f>Feuil1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1117,7 +1129,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$B$17</c:f>
+              <c:f>Feuil1!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1138,7 +1150,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$18:$A$26</c:f>
+              <c:f>Feuil1!$A$19:$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1173,7 +1185,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$18:$B$26</c:f>
+              <c:f>Feuil1!$B$19:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000000000</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1408,6 +1420,1246 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$E$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$35:$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dataset/buchanj-midwinter-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dataset/carman-farhorizons-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dataset/charlesworth-scene-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dataset/cheyneyp-darkbahama-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dataset/colby-champlain-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dataset/delamare-bumps-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dataset/delamare-lucy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dataset/delamare-myfanwy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dataset/delamare-penny-00-t.txt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$E$35:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.1764069616666673</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1661184740000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1463760693333329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0925157773333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1096795863333329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2055726689999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1075865880000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1068856123333326</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.2060067993333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5908-3748-8405-D4AD47A6C077}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$D$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Run 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$35:$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dataset/buchanj-midwinter-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dataset/carman-farhorizons-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dataset/charlesworth-scene-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dataset/cheyneyp-darkbahama-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dataset/colby-champlain-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dataset/delamare-bumps-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dataset/delamare-lucy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dataset/delamare-myfanwy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dataset/delamare-penny-00-t.txt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$D$35:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.1401026910000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2351261190000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.100013347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0667403569999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0992547630000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2036086030000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1313472290000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1528109879999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1256934459999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5908-3748-8405-D4AD47A6C077}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$C$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Run 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$35:$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dataset/buchanj-midwinter-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dataset/carman-farhorizons-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dataset/charlesworth-scene-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dataset/cheyneyp-darkbahama-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dataset/colby-champlain-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dataset/delamare-bumps-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dataset/delamare-lucy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dataset/delamare-myfanwy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dataset/delamare-penny-00-t.txt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$C$35:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.1739242819999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.131297161</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0878749719999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1885077610000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0648071410000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3050755690000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1127064899999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0202753280000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3084674329999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5908-3748-8405-D4AD47A6C077}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Run 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$35:$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dataset/buchanj-midwinter-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dataset/carman-farhorizons-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dataset/charlesworth-scene-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dataset/cheyneyp-darkbahama-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dataset/colby-champlain-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dataset/delamare-bumps-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dataset/delamare-lucy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dataset/delamare-myfanwy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dataset/delamare-penny-00-t.txt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$35:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.2151939120000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1319321420000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2512398889999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0222992140000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1649768549999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.1080338349999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0787060449999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1475705209999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1838595190000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5908-3748-8405-D4AD47A6C077}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1462101456"/>
+        <c:axId val="1462103104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1462101456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1462103104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1462103104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1462101456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$E$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$52:$A$60</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dataset/buchanj-midwinter-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dataset/carman-farhorizons-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dataset/charlesworth-scene-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dataset/cheyneyp-darkbahama-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dataset/colby-champlain-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dataset/delamare-bumps-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dataset/delamare-lucy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dataset/delamare-myfanwy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dataset/delamare-penny-00-t.txt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$E$52:$E$60</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.3256107653333329</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9471788630000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9950445393333345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9722562046666665</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9677380273333336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9576802133333331</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0049959006666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9627306289999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.031836274333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0123-4848-9967-90AAFA907D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$D$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Run 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$52:$A$60</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dataset/buchanj-midwinter-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dataset/carman-farhorizons-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dataset/charlesworth-scene-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dataset/cheyneyp-darkbahama-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dataset/colby-champlain-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dataset/delamare-bumps-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dataset/delamare-lucy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dataset/delamare-myfanwy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dataset/delamare-penny-00-t.txt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$D$52:$D$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.9287106070000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8210496899999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0652939960000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9107943089999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0426316370000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8449991529999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0346225819999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9455976819999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0945518009999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0123-4848-9967-90AAFA907D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$C$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Run 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$52:$A$60</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dataset/buchanj-midwinter-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dataset/carman-farhorizons-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dataset/charlesworth-scene-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dataset/cheyneyp-darkbahama-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dataset/colby-champlain-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dataset/delamare-bumps-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dataset/delamare-lucy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dataset/delamare-myfanwy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dataset/delamare-penny-00-t.txt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$C$52:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.9730640179999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9942549959999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9596657520000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.9732401050000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9154397850000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1194469199999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9254368179999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.0111523309999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9892243350000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0123-4848-9967-90AAFA907D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Run 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$52:$A$60</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>dataset/buchanj-midwinter-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dataset/carman-farhorizons-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dataset/charlesworth-scene-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dataset/cheyneyp-darkbahama-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>dataset/colby-champlain-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dataset/delamare-bumps-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dataset/delamare-lucy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dataset/delamare-myfanwy-00-t.txt</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dataset/delamare-penny-00-t.txt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$52:$B$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.0750576709999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0262319030000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9601738700000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0327342000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9451426600000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9085945669999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0549283020000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.9314418739999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0117326870000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0123-4848-9967-90AAFA907D65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1466060528"/>
+        <c:axId val="1466062176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1466060528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1466062176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1466062176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1466060528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1488,6 +2740,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -2498,20 +3830,1030 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>501650</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2538,16 +4880,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2567,6 +4909,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFFD7F70-CFD9-6242-9413-BB3CDB5F7048}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Graphique 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42C443D5-E5ED-7741-9053-D3307DF1DE5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2872,10 +5286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB69A3FF-A957-ED4E-8684-C1C50872F261}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2885,361 +5299,739 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
+      <c r="A1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.141628747</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.13906090600000001</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.13832148499999999</v>
-      </c>
-      <c r="E2" s="2">
-        <f>AVERAGE(B2:D2)</f>
-        <v>0.13967037933333334</v>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>2.1731005000000001E-2</v>
+        <v>0.141628747</v>
       </c>
       <c r="C3" s="2">
-        <v>1.9801329999999999E-2</v>
+        <v>0.13906090600000001</v>
       </c>
       <c r="D3" s="2">
-        <v>1.9296818E-2</v>
+        <v>0.13832148499999999</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E10" si="0">AVERAGE(B3:D3)</f>
-        <v>2.0276384333333335E-2</v>
+        <f>AVERAGE(B3:D3)</f>
+        <v>0.13967037933333334</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>6.7377012999999999E-2</v>
+        <v>2.1731005000000001E-2</v>
       </c>
       <c r="C4" s="2">
-        <v>6.7273875999999996E-2</v>
+        <v>1.9801329999999999E-2</v>
       </c>
       <c r="D4" s="2">
-        <v>6.7285640999999993E-2</v>
+        <v>1.9296818E-2</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>6.7312176666666668E-2</v>
+        <f t="shared" ref="E4:E11" si="0">AVERAGE(B4:D4)</f>
+        <v>2.0276384333333335E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>0.124537699</v>
+        <v>6.7377012999999999E-2</v>
       </c>
       <c r="C5" s="2">
-        <v>0.125759285</v>
+        <v>6.7273875999999996E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>0.12383395699999999</v>
+        <v>6.7285640999999993E-2</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="0"/>
-        <v>0.12471031366666667</v>
+        <v>6.7312176666666668E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>5.0038051E-2</v>
+        <v>0.124537699</v>
       </c>
       <c r="C6" s="2">
-        <v>5.0453524999999999E-2</v>
+        <v>0.125759285</v>
       </c>
       <c r="D6" s="2">
-        <v>4.6867387000000003E-2</v>
+        <v>0.12383395699999999</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>4.9119654333333339E-2</v>
+        <v>0.12471031366666667</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>1.7682243E-2</v>
+        <v>5.0038051E-2</v>
       </c>
       <c r="C7" s="2">
-        <v>1.8217015999999999E-2</v>
+        <v>5.0453524999999999E-2</v>
       </c>
       <c r="D7" s="2">
-        <v>1.6386016E-2</v>
+        <v>4.6867387000000003E-2</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>1.7428425000000001E-2</v>
+        <v>4.9119654333333339E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>1.8320125999999999E-2</v>
+        <v>1.7682243E-2</v>
       </c>
       <c r="C8" s="2">
-        <v>1.8725565999999999E-2</v>
+        <v>1.8217015999999999E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>1.8416485999999999E-2</v>
+        <v>1.6386016E-2</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>1.8487392666666668E-2</v>
+        <v>1.7428425000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
-        <v>1.7057241000000001E-2</v>
+        <v>1.8320125999999999E-2</v>
       </c>
       <c r="C9" s="2">
-        <v>1.7019680999999998E-2</v>
+        <v>1.8725565999999999E-2</v>
       </c>
       <c r="D9" s="2">
-        <v>1.6178828999999999E-2</v>
+        <v>1.8416485999999999E-2</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>1.6751916999999998E-2</v>
+        <v>1.8487392666666668E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>1.2604802999999999E-2</v>
+        <v>1.7057241000000001E-2</v>
       </c>
       <c r="C10" s="2">
-        <v>1.1556673999999999E-2</v>
+        <v>1.7019680999999998E-2</v>
       </c>
       <c r="D10" s="2">
-        <v>1.4607197000000001E-2</v>
+        <v>1.6178828999999999E-2</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="0"/>
+        <v>1.6751916999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.2604802999999999E-2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.1556673999999999E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.4607197000000001E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
         <v>1.2922891333333334E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>13</v>
+      <c r="A17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="3">
-        <v>3.5855428539999998</v>
-      </c>
-      <c r="C18" s="3">
-        <v>3.639901493</v>
-      </c>
-      <c r="D18" s="3">
-        <v>3.6099407800000001</v>
-      </c>
-      <c r="E18" s="2">
-        <f>AVERAGE(B18:D18)</f>
-        <v>3.6117950423333336</v>
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3.6351796470000002</v>
+        <v>0</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3.5855428539999998</v>
       </c>
       <c r="C19" s="3">
-        <v>3.6193401280000002</v>
+        <v>3.639901493</v>
       </c>
       <c r="D19" s="3">
-        <v>3.6221697449999999</v>
+        <v>3.6099407800000001</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" ref="E19:E26" si="1">AVERAGE(B19:D19)</f>
-        <v>3.6255631733333331</v>
+        <f>AVERAGE(B19:D19)</f>
+        <v>3.6117950423333336</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="3">
-        <v>3.5988001879999998</v>
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3.6351796470000002</v>
       </c>
       <c r="C20" s="3">
-        <v>3.61007072</v>
+        <v>3.6193401280000002</v>
       </c>
       <c r="D20" s="3">
-        <v>3.585876254</v>
+        <v>3.6221697449999999</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>3.5982490540000001</v>
+        <f t="shared" ref="E20:E27" si="1">AVERAGE(B20:D20)</f>
+        <v>3.6255631733333331</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="3">
-        <v>3.588466307</v>
+        <v>3.5988001879999998</v>
       </c>
       <c r="C21" s="3">
-        <v>3.6443139960000002</v>
+        <v>3.61007072</v>
       </c>
       <c r="D21" s="3">
-        <v>3.6039717310000001</v>
+        <v>3.585876254</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
-        <v>3.6122506780000001</v>
+        <v>3.5982490540000001</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" s="3">
-        <v>3.6326618009999998</v>
+        <v>3.588466307</v>
       </c>
       <c r="C22" s="3">
-        <v>3.6061054559999999</v>
+        <v>3.6443139960000002</v>
       </c>
       <c r="D22" s="3">
-        <v>3.6187007229999999</v>
+        <v>3.6039717310000001</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="1"/>
-        <v>3.619155993333333</v>
+        <v>3.6122506780000001</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="3">
-        <v>3.6041125869999999</v>
+        <v>3.6326618009999998</v>
       </c>
       <c r="C23" s="3">
-        <v>3.6066343920000001</v>
+        <v>3.6061054559999999</v>
       </c>
       <c r="D23" s="3">
-        <v>3.595871652</v>
+        <v>3.6187007229999999</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="1"/>
-        <v>3.6022062103333332</v>
+        <v>3.619155993333333</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="3">
-        <v>3.6136838760000001</v>
+        <v>3.6041125869999999</v>
       </c>
       <c r="C24" s="3">
-        <v>3.6234291650000001</v>
+        <v>3.6066343920000001</v>
       </c>
       <c r="D24" s="3">
-        <v>3.6273268330000001</v>
+        <v>3.595871652</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="1"/>
-        <v>3.6214799580000001</v>
+        <v>3.6022062103333332</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="3">
-        <v>3.592173893</v>
+        <v>3.6136838760000001</v>
       </c>
       <c r="C25" s="3">
-        <v>3.59800545</v>
+        <v>3.6234291650000001</v>
       </c>
       <c r="D25" s="3">
-        <v>3.6341224780000001</v>
+        <v>3.6273268330000001</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="1"/>
-        <v>3.6081006070000003</v>
+        <v>3.6214799580000001</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" s="3">
-        <v>3.644058931</v>
+        <v>3.592173893</v>
       </c>
       <c r="C26" s="3">
-        <v>3.6462254409999999</v>
+        <v>3.59800545</v>
       </c>
       <c r="D26" s="3">
-        <v>3.643883604</v>
+        <v>3.6341224780000001</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
+        <v>3.6081006070000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="3">
+        <v>3.644058931</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3.6462254409999999</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3.643883604</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
         <v>3.6447226586666672</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="3">
+        <v>4.2151939120000002</v>
+      </c>
+      <c r="C35" s="3">
+        <v>4.1739242819999998</v>
+      </c>
+      <c r="D35" s="3">
+        <v>4.1401026910000001</v>
+      </c>
+      <c r="E35" s="2">
+        <f>AVERAGE(B35:D35)</f>
+        <v>4.1764069616666673</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3">
+        <v>4.1319321420000001</v>
+      </c>
+      <c r="C36" s="3">
+        <v>4.131297161</v>
+      </c>
+      <c r="D36" s="3">
+        <v>4.2351261190000002</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" ref="E36:E43" si="2">AVERAGE(B36:D36)</f>
+        <v>4.1661184740000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="3">
+        <v>4.2512398889999998</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4.0878749719999998</v>
+      </c>
+      <c r="D37" s="3">
+        <v>4.100013347</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="2"/>
+        <v>4.1463760693333329</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="3">
+        <v>4.0222992140000002</v>
+      </c>
+      <c r="C38" s="3">
+        <v>4.1885077610000003</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4.0667403569999996</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="2"/>
+        <v>4.0925157773333334</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="3">
+        <v>4.1649768549999999</v>
+      </c>
+      <c r="C39" s="3">
+        <v>4.0648071410000002</v>
+      </c>
+      <c r="D39" s="3">
+        <v>4.0992547630000002</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="2"/>
+        <v>4.1096795863333329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="3">
+        <v>4.1080338349999996</v>
+      </c>
+      <c r="C40" s="3">
+        <v>4.3050755690000004</v>
+      </c>
+      <c r="D40" s="3">
+        <v>4.2036086030000002</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="2"/>
+        <v>4.2055726689999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="3">
+        <v>4.0787060449999997</v>
+      </c>
+      <c r="C41" s="3">
+        <v>4.1127064899999999</v>
+      </c>
+      <c r="D41" s="3">
+        <v>4.1313472290000002</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="2"/>
+        <v>4.1075865880000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3">
+        <v>4.1475705209999996</v>
+      </c>
+      <c r="C42" s="3">
+        <v>4.0202753280000003</v>
+      </c>
+      <c r="D42" s="3">
+        <v>4.1528109879999997</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="2"/>
+        <v>4.1068856123333326</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="3">
+        <v>4.1838595190000003</v>
+      </c>
+      <c r="C43" s="3">
+        <v>4.3084674329999997</v>
+      </c>
+      <c r="D43" s="3">
+        <v>4.1256934459999997</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="2"/>
+        <v>4.2060067993333332</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="3">
+        <v>6.0750576709999997</v>
+      </c>
+      <c r="C52" s="3">
+        <v>4.9730640179999996</v>
+      </c>
+      <c r="D52" s="3">
+        <v>4.9287106070000002</v>
+      </c>
+      <c r="E52" s="2">
+        <f>AVERAGE(B52:D52)</f>
+        <v>5.3256107653333329</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="3">
+        <v>5.0262319030000002</v>
+      </c>
+      <c r="C53" s="3">
+        <v>4.9942549959999996</v>
+      </c>
+      <c r="D53" s="3">
+        <v>4.8210496899999997</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" ref="E53:E60" si="3">AVERAGE(B53:D53)</f>
+        <v>4.9471788630000004</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="3">
+        <v>4.9601738700000002</v>
+      </c>
+      <c r="C54" s="3">
+        <v>4.9596657520000003</v>
+      </c>
+      <c r="D54" s="3">
+        <v>5.0652939960000003</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="3"/>
+        <v>4.9950445393333345</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="3">
+        <v>5.0327342000000002</v>
+      </c>
+      <c r="C55" s="3">
+        <v>4.9732401050000004</v>
+      </c>
+      <c r="D55" s="3">
+        <v>4.9107943089999999</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="3"/>
+        <v>4.9722562046666665</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="3">
+        <v>4.9451426600000001</v>
+      </c>
+      <c r="C56" s="3">
+        <v>4.9154397850000002</v>
+      </c>
+      <c r="D56" s="3">
+        <v>5.0426316370000004</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="3"/>
+        <v>4.9677380273333336</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="3">
+        <v>4.9085945669999997</v>
+      </c>
+      <c r="C57" s="3">
+        <v>5.1194469199999997</v>
+      </c>
+      <c r="D57" s="3">
+        <v>4.8449991529999998</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="3"/>
+        <v>4.9576802133333331</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="3">
+        <v>5.0549283020000004</v>
+      </c>
+      <c r="C58" s="3">
+        <v>4.9254368179999997</v>
+      </c>
+      <c r="D58" s="3">
+        <v>5.0346225819999999</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="3"/>
+        <v>5.0049959006666667</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="3">
+        <v>4.9314418739999999</v>
+      </c>
+      <c r="C59" s="3">
+        <v>5.0111523309999999</v>
+      </c>
+      <c r="D59" s="3">
+        <v>4.9455976819999998</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="3"/>
+        <v>4.9627306289999993</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="3">
+        <v>5.0117326870000003</v>
+      </c>
+      <c r="C60" s="3">
+        <v>4.9892243350000003</v>
+      </c>
+      <c r="D60" s="3">
+        <v>5.0945518009999997</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="3"/>
+        <v>5.031836274333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel with good data
</commit_message>
<xml_diff>
--- a/TP2/expermiments.xlsx
+++ b/TP2/expermiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beding/Polytechnique/LOG8415E/Laboratoires/LOG8415/TP2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6343AB31-BD71-DB45-983B-AA0B4783DAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72553627-3A50-6F42-9313-13265B804535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17920" yWindow="500" windowWidth="17920" windowHeight="20400" xr2:uid="{96923936-A141-844A-8B93-6ABFCA660DBE}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -141,8 +141,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,7 +244,7 @@
             <c:numRef>
               <c:f>Feuil1!$E$3:$E$11</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.13967037933333334</c:v>
@@ -345,7 +345,7 @@
             <c:numRef>
               <c:f>Feuil1!$D$3:$D$11</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.13832148499999999</c:v>
@@ -446,7 +446,7 @@
             <c:numRef>
               <c:f>Feuil1!$C$3:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.13906090600000001</c:v>
@@ -547,7 +547,7 @@
             <c:numRef>
               <c:f>Feuil1!$B$3:$B$11</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.141628747</c:v>
@@ -864,34 +864,34 @@
             <c:numRef>
               <c:f>Feuil1!$E$19:$E$27</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3.6117950423333336</c:v>
+                  <c:v>1.2226666666666668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6255631733333331</c:v>
+                  <c:v>1.2450000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5982490540000001</c:v>
+                  <c:v>1.2163333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6122506780000001</c:v>
+                  <c:v>1.2126666666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.619155993333333</c:v>
+                  <c:v>1.2306666666666668</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6022062103333332</c:v>
+                  <c:v>1.4776999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6214799580000001</c:v>
+                  <c:v>1.2260000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6081006070000003</c:v>
+                  <c:v>1.2236666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6447226586666672</c:v>
+                  <c:v>1.2203333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -965,34 +965,34 @@
             <c:numRef>
               <c:f>Feuil1!$D$19:$D$27</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3.6099407800000001</c:v>
+                  <c:v>1.222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6221697449999999</c:v>
+                  <c:v>1.2609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.585876254</c:v>
+                  <c:v>1.2170000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6039717310000001</c:v>
+                  <c:v>1.2110000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6187007229999999</c:v>
+                  <c:v>1.2190000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.595871652</c:v>
+                  <c:v>1.2509999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6273268330000001</c:v>
+                  <c:v>1.2170000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6341224780000001</c:v>
+                  <c:v>1.2230000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.643883604</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1066,34 +1066,34 @@
             <c:numRef>
               <c:f>Feuil1!$C$19:$C$27</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3.639901493</c:v>
+                  <c:v>1.2250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6193401280000002</c:v>
+                  <c:v>1.2350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.61007072</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6443139960000002</c:v>
+                  <c:v>1.212</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6061054559999999</c:v>
+                  <c:v>1.236</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6066343920000001</c:v>
+                  <c:v>1.2829999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.6234291650000001</c:v>
+                  <c:v>1.2370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.59800545</c:v>
+                  <c:v>1.2230000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6462254409999999</c:v>
+                  <c:v>1.23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1167,34 +1167,34 @@
             <c:numRef>
               <c:f>Feuil1!$B$19:$B$27</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>3.5855428539999998</c:v>
+                <c:pt idx="0">
+                  <c:v>1.2210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6351796470000002</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>3.5988001879999998</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>3.588466307</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>3.6326618009999998</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>3.6041125869999999</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>3.6136838760000001</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>3.592173893</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>3.644058931</c:v>
+                  <c:v>1.2390000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.212</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8991</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2210000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1484,34 +1484,34 @@
             <c:numRef>
               <c:f>Feuil1!$E$35:$E$43</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.1764069616666673</c:v>
+                  <c:v>1.0683333333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1661184740000001</c:v>
+                  <c:v>1.0640000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.1463760693333329</c:v>
+                  <c:v>1.0683333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0925157773333334</c:v>
+                  <c:v>1.0623333333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1096795863333329</c:v>
+                  <c:v>1.0650000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2055726689999995</c:v>
+                  <c:v>1.0626666666666666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1075865880000002</c:v>
+                  <c:v>1.0839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1068856123333326</c:v>
+                  <c:v>1.0643333333333336</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.2060067993333332</c:v>
+                  <c:v>1.2966666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1585,34 +1585,34 @@
             <c:numRef>
               <c:f>Feuil1!$D$35:$D$43</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.1401026910000001</c:v>
+                  <c:v>1.0629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2351261190000002</c:v>
+                  <c:v>1.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.100013347</c:v>
+                  <c:v>1.0609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0667403569999996</c:v>
+                  <c:v>1.0589999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0992547630000002</c:v>
+                  <c:v>1.0740000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2036086030000002</c:v>
+                  <c:v>1.0609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1313472290000002</c:v>
+                  <c:v>1.085</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1528109879999997</c:v>
+                  <c:v>1.0620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1256934459999997</c:v>
+                  <c:v>1.095</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1686,34 +1686,34 @@
             <c:numRef>
               <c:f>Feuil1!$C$35:$C$43</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.1739242819999998</c:v>
+                  <c:v>1.0680000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.131297161</c:v>
+                  <c:v>1.0629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0878749719999998</c:v>
+                  <c:v>1.081</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1885077610000003</c:v>
+                  <c:v>1.07</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0648071410000002</c:v>
+                  <c:v>1.0609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3050755690000004</c:v>
+                  <c:v>1.06</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1127064899999999</c:v>
+                  <c:v>1.083</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0202753280000003</c:v>
+                  <c:v>1.0609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3084674329999997</c:v>
+                  <c:v>1.105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1787,34 +1787,34 @@
             <c:numRef>
               <c:f>Feuil1!$B$35:$B$43</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.2151939120000002</c:v>
+                  <c:v>1.0740000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1319321420000001</c:v>
+                  <c:v>1.0589999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2512398889999998</c:v>
+                  <c:v>1.0629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0222992140000002</c:v>
+                  <c:v>1.0580000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1649768549999999</c:v>
+                  <c:v>1.06</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1080338349999996</c:v>
+                  <c:v>1.0669999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0787060449999997</c:v>
+                  <c:v>1.0840000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1475705209999996</c:v>
+                  <c:v>1.07</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1838595190000003</c:v>
+                  <c:v>1.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2104,34 +2104,34 @@
             <c:numRef>
               <c:f>Feuil1!$E$52:$E$60</c:f>
               <c:numCache>
-                <c:formatCode>0.000000000</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5.3256107653333329</c:v>
+                  <c:v>0.39366666666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9471788630000004</c:v>
+                  <c:v>0.126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9950445393333345</c:v>
+                  <c:v>0.23399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9722562046666665</c:v>
+                  <c:v>0.14333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9677380273333336</c:v>
+                  <c:v>0.17733333333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9576802133333331</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0049959006666667</c:v>
+                  <c:v>0.2243333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9627306289999993</c:v>
+                  <c:v>0.14300000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.031836274333334</c:v>
+                  <c:v>0.52900000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2205,34 +2205,34 @@
             <c:numRef>
               <c:f>Feuil1!$D$52:$D$60</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.9287106070000002</c:v>
+                  <c:v>0.35599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8210496899999997</c:v>
+                  <c:v>0.10299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0652939960000003</c:v>
+                  <c:v>0.19800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9107943089999999</c:v>
+                  <c:v>0.13900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0426316370000004</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8449991529999998</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0346225819999999</c:v>
+                  <c:v>0.20899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9455976819999998</c:v>
+                  <c:v>0.13800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0945518009999997</c:v>
+                  <c:v>0.21199999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2306,34 +2306,34 @@
             <c:numRef>
               <c:f>Feuil1!$C$52:$C$60</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.9730640179999996</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9942549959999996</c:v>
+                  <c:v>0.11600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9596657520000003</c:v>
+                  <c:v>0.25600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9732401050000004</c:v>
+                  <c:v>0.13400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9154397850000002</c:v>
+                  <c:v>0.20300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1194469199999997</c:v>
+                  <c:v>0.13700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9254368179999997</c:v>
+                  <c:v>0.23699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0111523309999999</c:v>
+                  <c:v>0.153</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.9892243350000003</c:v>
+                  <c:v>0.26600000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2407,34 +2407,34 @@
             <c:numRef>
               <c:f>Feuil1!$B$52:$B$60</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6.0750576709999997</c:v>
+                  <c:v>0.40500000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0262319030000002</c:v>
+                  <c:v>0.159</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9601738700000002</c:v>
+                  <c:v>0.248</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0327342000000002</c:v>
+                  <c:v>0.157</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9451426600000001</c:v>
+                  <c:v>0.17899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9085945669999997</c:v>
+                  <c:v>0.17299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0549283020000004</c:v>
+                  <c:v>0.22700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9314418739999999</c:v>
+                  <c:v>0.13800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0117326870000003</c:v>
+                  <c:v>1.109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4860,16 +4860,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4896,16 +4896,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4932,16 +4932,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4964,6 +4964,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>10694</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{929817E0-7549-014B-A84B-179283E03620}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="28460700" y="17043400"/>
+          <a:ext cx="7772400" cy="7351294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5268,8 +5312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB69A3FF-A957-ED4E-8684-C1C50872F261}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5458,7 +5502,7 @@
         <v>1.4607197000000001E-2</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B11:D11)</f>
         <v>1.2922891333333334E-2</v>
       </c>
     </row>
@@ -5489,17 +5533,17 @@
         <v>0</v>
       </c>
       <c r="B19" s="3">
-        <v>3.5855428539999998</v>
+        <v>1.2210000000000001</v>
       </c>
       <c r="C19" s="3">
-        <v>3.639901493</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="D19" s="3">
-        <v>3.6099407800000001</v>
+        <v>1.222</v>
       </c>
       <c r="E19" s="2">
         <f>AVERAGE(B19:D19)</f>
-        <v>3.6117950423333336</v>
+        <v>1.2226666666666668</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -5507,17 +5551,17 @@
         <v>1</v>
       </c>
       <c r="B20" s="2">
-        <v>3.6351796470000002</v>
+        <v>1.2390000000000001</v>
       </c>
       <c r="C20" s="3">
-        <v>3.6193401280000002</v>
+        <v>1.2350000000000001</v>
       </c>
       <c r="D20" s="3">
-        <v>3.6221697449999999</v>
+        <v>1.2609999999999999</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ref="E20:E27" si="1">AVERAGE(B20:D20)</f>
-        <v>3.6255631733333331</v>
+        <v>1.2450000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -5525,17 +5569,17 @@
         <v>2</v>
       </c>
       <c r="B21" s="3">
-        <v>3.5988001879999998</v>
+        <v>1.212</v>
       </c>
       <c r="C21" s="3">
-        <v>3.61007072</v>
+        <v>1.22</v>
       </c>
       <c r="D21" s="3">
-        <v>3.585876254</v>
+        <v>1.2170000000000001</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
-        <v>3.5982490540000001</v>
+        <v>1.2163333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -5543,17 +5587,17 @@
         <v>3</v>
       </c>
       <c r="B22" s="3">
-        <v>3.588466307</v>
+        <v>1.2150000000000001</v>
       </c>
       <c r="C22" s="3">
-        <v>3.6443139960000002</v>
+        <v>1.212</v>
       </c>
       <c r="D22" s="3">
-        <v>3.6039717310000001</v>
+        <v>1.2110000000000001</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="1"/>
-        <v>3.6122506780000001</v>
+        <v>1.2126666666666666</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -5561,17 +5605,17 @@
         <v>4</v>
       </c>
       <c r="B23" s="3">
-        <v>3.6326618009999998</v>
+        <v>1.2370000000000001</v>
       </c>
       <c r="C23" s="3">
-        <v>3.6061054559999999</v>
+        <v>1.236</v>
       </c>
       <c r="D23" s="3">
-        <v>3.6187007229999999</v>
+        <v>1.2190000000000001</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="1"/>
-        <v>3.619155993333333</v>
+        <v>1.2306666666666668</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -5579,17 +5623,17 @@
         <v>5</v>
       </c>
       <c r="B24" s="3">
-        <v>3.6041125869999999</v>
+        <v>1.8991</v>
       </c>
       <c r="C24" s="3">
-        <v>3.6066343920000001</v>
+        <v>1.2829999999999999</v>
       </c>
       <c r="D24" s="3">
-        <v>3.595871652</v>
+        <v>1.2509999999999999</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="1"/>
-        <v>3.6022062103333332</v>
+        <v>1.4776999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -5597,17 +5641,17 @@
         <v>6</v>
       </c>
       <c r="B25" s="3">
-        <v>3.6136838760000001</v>
+        <v>1.224</v>
       </c>
       <c r="C25" s="3">
-        <v>3.6234291650000001</v>
+        <v>1.2370000000000001</v>
       </c>
       <c r="D25" s="3">
-        <v>3.6273268330000001</v>
+        <v>1.2170000000000001</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="1"/>
-        <v>3.6214799580000001</v>
+        <v>1.2260000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -5615,17 +5659,17 @@
         <v>7</v>
       </c>
       <c r="B26" s="3">
-        <v>3.592173893</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="C26" s="3">
-        <v>3.59800545</v>
+        <v>1.2230000000000001</v>
       </c>
       <c r="D26" s="3">
-        <v>3.6341224780000001</v>
+        <v>1.2230000000000001</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
-        <v>3.6081006070000003</v>
+        <v>1.2236666666666667</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -5633,17 +5677,17 @@
         <v>8</v>
       </c>
       <c r="B27" s="3">
-        <v>3.644058931</v>
+        <v>1.2210000000000001</v>
       </c>
       <c r="C27" s="3">
-        <v>3.6462254409999999</v>
+        <v>1.23</v>
       </c>
       <c r="D27" s="3">
-        <v>3.643883604</v>
+        <v>1.21</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
-        <v>3.6447226586666672</v>
+        <v>1.2203333333333333</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -5673,17 +5717,17 @@
         <v>0</v>
       </c>
       <c r="B35" s="3">
-        <v>4.2151939120000002</v>
+        <v>1.0740000000000001</v>
       </c>
       <c r="C35" s="3">
-        <v>4.1739242819999998</v>
+        <v>1.0680000000000001</v>
       </c>
       <c r="D35" s="3">
-        <v>4.1401026910000001</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="E35" s="2">
         <f>AVERAGE(B35:D35)</f>
-        <v>4.1764069616666673</v>
+        <v>1.0683333333333334</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -5691,17 +5735,17 @@
         <v>1</v>
       </c>
       <c r="B36" s="3">
-        <v>4.1319321420000001</v>
+        <v>1.0589999999999999</v>
       </c>
       <c r="C36" s="3">
-        <v>4.131297161</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="D36" s="3">
-        <v>4.2351261190000002</v>
+        <v>1.07</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" ref="E36:E43" si="2">AVERAGE(B36:D36)</f>
-        <v>4.1661184740000001</v>
+        <f>AVERAGE(B36:D36)</f>
+        <v>1.0640000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -5709,17 +5753,17 @@
         <v>2</v>
       </c>
       <c r="B37" s="3">
-        <v>4.2512398889999998</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="C37" s="3">
-        <v>4.0878749719999998</v>
+        <v>1.081</v>
       </c>
       <c r="D37" s="3">
-        <v>4.100013347</v>
+        <v>1.0609999999999999</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="2"/>
-        <v>4.1463760693333329</v>
+        <f t="shared" ref="E36:E43" si="2">AVERAGE(B37:D37)</f>
+        <v>1.0683333333333334</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -5727,17 +5771,17 @@
         <v>3</v>
       </c>
       <c r="B38" s="3">
-        <v>4.0222992140000002</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="C38" s="3">
-        <v>4.1885077610000003</v>
+        <v>1.07</v>
       </c>
       <c r="D38" s="3">
-        <v>4.0667403569999996</v>
+        <v>1.0589999999999999</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="2"/>
-        <v>4.0925157773333334</v>
+        <v>1.0623333333333334</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -5745,17 +5789,17 @@
         <v>4</v>
       </c>
       <c r="B39" s="3">
-        <v>4.1649768549999999</v>
+        <v>1.06</v>
       </c>
       <c r="C39" s="3">
-        <v>4.0648071410000002</v>
+        <v>1.0609999999999999</v>
       </c>
       <c r="D39" s="3">
-        <v>4.0992547630000002</v>
+        <v>1.0740000000000001</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="2"/>
-        <v>4.1096795863333329</v>
+        <v>1.0650000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -5763,17 +5807,17 @@
         <v>5</v>
       </c>
       <c r="B40" s="3">
-        <v>4.1080338349999996</v>
+        <v>1.0669999999999999</v>
       </c>
       <c r="C40" s="3">
-        <v>4.3050755690000004</v>
+        <v>1.06</v>
       </c>
       <c r="D40" s="3">
-        <v>4.2036086030000002</v>
+        <v>1.0609999999999999</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="2"/>
-        <v>4.2055726689999995</v>
+        <v>1.0626666666666666</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -5781,17 +5825,17 @@
         <v>6</v>
       </c>
       <c r="B41" s="3">
-        <v>4.0787060449999997</v>
+        <v>1.0840000000000001</v>
       </c>
       <c r="C41" s="3">
-        <v>4.1127064899999999</v>
+        <v>1.083</v>
       </c>
       <c r="D41" s="3">
-        <v>4.1313472290000002</v>
+        <v>1.085</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="2"/>
-        <v>4.1075865880000002</v>
+        <v>1.0839999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -5799,17 +5843,17 @@
         <v>7</v>
       </c>
       <c r="B42" s="3">
-        <v>4.1475705209999996</v>
+        <v>1.07</v>
       </c>
       <c r="C42" s="3">
-        <v>4.0202753280000003</v>
+        <v>1.0609999999999999</v>
       </c>
       <c r="D42" s="3">
-        <v>4.1528109879999997</v>
+        <v>1.0620000000000001</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="2"/>
-        <v>4.1068856123333326</v>
+        <v>1.0643333333333336</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -5817,17 +5861,17 @@
         <v>8</v>
       </c>
       <c r="B43" s="3">
-        <v>4.1838595190000003</v>
+        <v>1.69</v>
       </c>
       <c r="C43" s="3">
-        <v>4.3084674329999997</v>
+        <v>1.105</v>
       </c>
       <c r="D43" s="3">
-        <v>4.1256934459999997</v>
+        <v>1.095</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="2"/>
-        <v>4.2060067993333332</v>
+        <v>1.2966666666666666</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -5857,17 +5901,17 @@
         <v>0</v>
       </c>
       <c r="B52" s="3">
-        <v>6.0750576709999997</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="C52" s="3">
-        <v>4.9730640179999996</v>
+        <v>0.42</v>
       </c>
       <c r="D52" s="3">
-        <v>4.9287106070000002</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="E52" s="2">
         <f>AVERAGE(B52:D52)</f>
-        <v>5.3256107653333329</v>
+        <v>0.39366666666666666</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -5875,17 +5919,17 @@
         <v>1</v>
       </c>
       <c r="B53" s="3">
-        <v>5.0262319030000002</v>
+        <v>0.159</v>
       </c>
       <c r="C53" s="3">
-        <v>4.9942549959999996</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="D53" s="3">
-        <v>4.8210496899999997</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" ref="E53:E60" si="3">AVERAGE(B53:D53)</f>
-        <v>4.9471788630000004</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -5893,17 +5937,17 @@
         <v>2</v>
       </c>
       <c r="B54" s="3">
-        <v>4.9601738700000002</v>
+        <v>0.248</v>
       </c>
       <c r="C54" s="3">
-        <v>4.9596657520000003</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="D54" s="3">
-        <v>5.0652939960000003</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="E54" s="2">
         <f t="shared" si="3"/>
-        <v>4.9950445393333345</v>
+        <v>0.23399999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -5911,17 +5955,17 @@
         <v>3</v>
       </c>
       <c r="B55" s="3">
-        <v>5.0327342000000002</v>
+        <v>0.157</v>
       </c>
       <c r="C55" s="3">
-        <v>4.9732401050000004</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="D55" s="3">
-        <v>4.9107943089999999</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="E55" s="2">
         <f t="shared" si="3"/>
-        <v>4.9722562046666665</v>
+        <v>0.14333333333333334</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -5929,17 +5973,17 @@
         <v>4</v>
       </c>
       <c r="B56" s="3">
-        <v>4.9451426600000001</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="C56" s="3">
-        <v>4.9154397850000002</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="D56" s="3">
-        <v>5.0426316370000004</v>
+        <v>0.15</v>
       </c>
       <c r="E56" s="2">
         <f t="shared" si="3"/>
-        <v>4.9677380273333336</v>
+        <v>0.17733333333333334</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -5947,17 +5991,17 @@
         <v>5</v>
       </c>
       <c r="B57" s="3">
-        <v>4.9085945669999997</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="C57" s="3">
-        <v>5.1194469199999997</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="D57" s="3">
-        <v>4.8449991529999998</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E57" s="2">
         <f t="shared" si="3"/>
-        <v>4.9576802133333331</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -5965,17 +6009,17 @@
         <v>6</v>
       </c>
       <c r="B58" s="3">
-        <v>5.0549283020000004</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="C58" s="3">
-        <v>4.9254368179999997</v>
+        <v>0.23699999999999999</v>
       </c>
       <c r="D58" s="3">
-        <v>5.0346225819999999</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="E58" s="2">
         <f t="shared" si="3"/>
-        <v>5.0049959006666667</v>
+        <v>0.2243333333333333</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -5983,17 +6027,17 @@
         <v>7</v>
       </c>
       <c r="B59" s="3">
-        <v>4.9314418739999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="C59" s="3">
-        <v>5.0111523309999999</v>
+        <v>0.153</v>
       </c>
       <c r="D59" s="3">
-        <v>4.9455976819999998</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="E59" s="2">
         <f t="shared" si="3"/>
-        <v>4.9627306289999993</v>
+        <v>0.14300000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -6001,17 +6045,17 @@
         <v>8</v>
       </c>
       <c r="B60" s="3">
-        <v>5.0117326870000003</v>
+        <v>1.109</v>
       </c>
       <c r="C60" s="3">
-        <v>4.9892243350000003</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="D60" s="3">
-        <v>5.0945518009999997</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="3"/>
-        <v>5.031836274333334</v>
+        <f>AVERAGE(B60:D60)</f>
+        <v>0.52900000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>